<commit_message>
RTL genomics library sample form
</commit_message>
<xml_diff>
--- a/Other/Transcriptomics/RNA_extractions.xlsx
+++ b/Other/Transcriptomics/RNA_extractions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_CellularMolecular_OA\Other\Transcriptomics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.gurr\Documents\Github_repositories\Airradians_CellularMolecular_OA\Other\Transcriptomics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F0D1F-CBAD-4D7E-BC6F-95BE88F07867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2757D6C9-2674-4A04-83E8-57DBE912A3F9}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="19416" windowHeight="11496"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,29 +491,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2EF53A-3697-4672-9A8D-6EDEAB17C2A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="63" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="63" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="2" customWidth="1"/>
-    <col min="5" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="2"/>
-    <col min="11" max="11" width="22.26953125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="8.77734375" style="2"/>
+    <col min="7" max="7" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" style="2"/>
+    <col min="11" max="11" width="22.21875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -572,7 +570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -595,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -618,7 +616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -641,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -664,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -687,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -710,7 +708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -733,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -756,7 +754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -779,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -802,7 +800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -825,7 +823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -848,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -871,7 +869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -894,7 +892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -917,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -940,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -973,7 +971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -996,7 +994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1065,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1203,7 +1201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1226,7 +1224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1247,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1270,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1295,7 +1293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1341,7 +1339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +1385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1433,7 +1431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1456,7 +1454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1479,7 +1477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -1548,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1594,7 +1592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
@@ -1639,7 +1637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1679,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>6</v>
       </c>
@@ -1726,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>6</v>
       </c>
@@ -1764,11 +1762,11 @@
         <v>48.6</v>
       </c>
       <c r="M50" s="4">
-        <f t="shared" ref="M49:M91" si="0">AVERAGE(K50:L50)</f>
+        <f t="shared" ref="M50:M91" si="0">AVERAGE(K50:L50)</f>
         <v>48.650000000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>6</v>
       </c>
@@ -1810,7 +1808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>6</v>
       </c>
@@ -1846,7 +1844,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1880,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1916,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
@@ -1954,7 +1952,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>6</v>
       </c>
@@ -2032,7 +2030,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="58" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
@@ -2077,7 +2075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2117,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="60" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
@@ -2161,7 +2159,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2201,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>6</v>
       </c>
@@ -2287,7 +2285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>6</v>
       </c>
@@ -2329,7 +2327,7 @@
         <v>33.650000000000006</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>6</v>
       </c>
@@ -2371,7 +2369,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>6</v>
       </c>
@@ -2413,7 +2411,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
@@ -2455,7 +2453,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>6</v>
       </c>
@@ -2497,7 +2495,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>6</v>
       </c>
@@ -2626,7 +2624,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
@@ -2671,7 +2669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2756,7 @@
         <v>41.650000000000006</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>6</v>
       </c>
@@ -2803,7 +2801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>6</v>
       </c>
@@ -2845,7 +2843,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="77" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>6</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>6</v>
       </c>
@@ -2929,7 +2927,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>6</v>
       </c>
@@ -2971,7 +2969,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
@@ -3016,7 +3014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>6</v>
       </c>
@@ -3061,7 +3059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>6</v>
       </c>
@@ -3097,7 +3095,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>6</v>
       </c>
@@ -3133,7 +3131,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>6</v>
       </c>
@@ -3169,7 +3167,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>6</v>
       </c>
@@ -3205,7 +3203,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>6</v>
       </c>
@@ -3247,7 +3245,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>6</v>
       </c>
@@ -3292,7 +3290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>6</v>
       </c>
@@ -3334,7 +3332,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -3379,7 +3377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>6</v>
       </c>
@@ -3421,7 +3419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>